<commit_message>
fix: validasi input, lokasi dosen management
</commit_message>
<xml_diff>
--- a/public/excel/template_admin.xlsx
+++ b/public/excel/template_admin.xlsx
@@ -440,5 +440,14 @@
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>